<commit_message>
Updated original excel files
Fixed the coefficients for the weigh of the SPF
</commit_message>
<xml_diff>
--- a/Data/Original Data/D2 LWA Crash Data.xlsx
+++ b/Data/Original Data/D2 LWA Crash Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault.sharepoint.com/sites/DataAnalyticsforCurveCrashesSpring2022/Shared Documents/General/Crash Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{7A16DA42-DEED-46F8-9822-F2BD64544967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E66EEC0-E8D1-40B7-A151-8516A7C8E577}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{7A16DA42-DEED-46F8-9822-F2BD64544967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A472A13-5F1C-4052-B972-E78E5C1D2837}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{524DC437-0BF5-4F4C-8031-0A4DE0B9EBF0}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
-    <pivotCache cacheId="39" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1323,10 +1323,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -16058,7 +16058,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34FF0675-2BD9-443B-AA98-432423259D65}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34FF0675-2BD9-443B-AA98-432423259D65}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="ES1:EU18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16221,7 +16221,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41BEAB96-6698-4910-9F74-3B3AFEBA9194}" name="PivotTable7" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41BEAB96-6698-4910-9F74-3B3AFEBA9194}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AA4:AD8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16441,7 +16441,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91E53CD8-EC4C-4C3E-BA7A-BF157D5A708D}" name="PivotTable6" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91E53CD8-EC4C-4C3E-BA7A-BF157D5A708D}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="S4:V9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16672,7 +16672,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8709ADE0-A902-4616-9902-6F3D8F188C5D}" name="PivotTable5" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8709ADE0-A902-4616-9902-6F3D8F188C5D}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J4:N10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16899,7 +16899,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66F1C9EA-B65D-4333-BBB8-A49886919643}" name="PivotTable3" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66F1C9EA-B65D-4333-BBB8-A49886919643}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -57640,8 +57640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA58A84-B0EF-4C65-8566-FEE0B8456301}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57668,46 +57668,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="S1" s="17" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="S1" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="17" t="s">
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="J2" s="13" t="s">
@@ -57905,16 +57905,16 @@
         <v>1</v>
       </c>
       <c r="W6">
-        <f>S6/3</f>
-        <v>0.66666666666666663</v>
+        <f>T6/3</f>
+        <v>0</v>
       </c>
       <c r="X6">
-        <f>T6/4</f>
-        <v>0</v>
+        <f>U6/4</f>
+        <v>0.25</v>
       </c>
       <c r="Y6">
         <f>IF(X6=0, 1, W6/X6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="14">
         <v>3</v>
@@ -57927,16 +57927,16 @@
         <v>1</v>
       </c>
       <c r="AE6">
-        <f>AA6/3</f>
-        <v>1</v>
+        <f>AB6/3</f>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <f>AB6/4</f>
-        <v>0</v>
+        <f>AC6/4</f>
+        <v>0.25</v>
       </c>
       <c r="AG6">
         <f>IF(AF6=0, 1, AE6/AF6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
@@ -58003,16 +58003,16 @@
         <v>3</v>
       </c>
       <c r="W7">
-        <f t="shared" ref="W7:W8" si="6">S7/3</f>
-        <v>1</v>
+        <f t="shared" ref="W7:W8" si="6">T7/3</f>
+        <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" ref="X7:X9" si="7">T7/4</f>
-        <v>0</v>
+        <f t="shared" ref="X7:X8" si="7">U7/4</f>
+        <v>0.75</v>
       </c>
       <c r="Y7">
-        <f t="shared" ref="Y7:Y9" si="8">IF(X7=0, 1, W7/X7)</f>
-        <v>1</v>
+        <f>IF(X7=0, 1, W7/X7)</f>
+        <v>0</v>
       </c>
       <c r="AA7" s="14">
         <v>4</v>
@@ -58025,16 +58025,16 @@
         <v>3</v>
       </c>
       <c r="AE7">
-        <f>AA7/3</f>
-        <v>1.3333333333333333</v>
+        <f>AB7/3</f>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <f t="shared" ref="AF7:AF9" si="9">AB7/4</f>
-        <v>0.75</v>
+        <f>AC7/4</f>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" ref="AG7:AG8" si="10">IF(AF7=0, 1, AE7/AF7)</f>
-        <v>1.7777777777777777</v>
+        <f t="shared" ref="AG7:AG8" si="8">IF(AF7=0, 1, AE7/AF7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -58104,15 +58104,15 @@
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>1.6666666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="X8">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="8"/>
-        <v>6.666666666666667</v>
+        <f t="shared" ref="Y7:Y8" si="9">IF(X8=0, 1, W8/X8)</f>
+        <v>1</v>
       </c>
       <c r="AA8" s="14" t="s">
         <v>328</v>
@@ -58128,15 +58128,15 @@
       </c>
       <c r="AE8" s="16">
         <f>SUM(AE6:AE7)</f>
-        <v>2.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="16">
         <f>SUM(AF6:AF7)</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AG8" s="16">
-        <f t="shared" si="10"/>
-        <v>3.1111111111111107</v>
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -58206,15 +58206,15 @@
       </c>
       <c r="W9" s="16">
         <f>SUM(W6:W8)</f>
-        <v>3.333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="X9" s="16">
         <f>SUM(X6:X8)</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="16">
         <f>IF(X9=0, 1, W9/X9)</f>
-        <v>13.333333333333332</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -58286,12 +58286,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58441,15 +58438,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4114F-5715-4E58-B4E5-37E54750F1CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D475958-A078-4CDC-BD7E-303003620B85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39631665-2ac6-4b14-83d9-84f76f5a0db8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -58473,17 +58481,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D475958-A078-4CDC-BD7E-303003620B85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4114F-5715-4E58-B4E5-37E54750F1CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39631665-2ac6-4b14-83d9-84f76f5a0db8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>